<commit_message>
Massive update - now includes call to entrainment mechanism
</commit_message>
<xml_diff>
--- a/automated_system/LogSync/data/LogSyncedResults/4_030817.xlsx
+++ b/automated_system/LogSync/data/LogSyncedResults/4_030817.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nikki\ASU_Research\NRI_Project\System\NRI_Git_Hub\automated_system\LogSync\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nikki\ASU_Research\NRI_Project\System\NRI_Git_Hub\automated_system\LogSync\data\LogSyncedResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="alldata" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">alldata!$A$1:$O$245</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -1348,13 +1351,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1955,7 +1958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2320,7 +2323,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2466,7 +2469,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2679,7 +2682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2825,7 +2828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2971,7 +2974,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3044,7 +3047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3111,7 +3114,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3178,7 +3181,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3321,7 +3324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3540,7 +3543,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3613,7 +3616,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3686,7 +3689,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3759,7 +3762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3826,7 +3829,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3893,7 +3896,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3960,7 +3963,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4027,7 +4030,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4094,7 +4097,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4228,7 +4231,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4374,7 +4377,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4447,7 +4450,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -4520,7 +4523,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4593,7 +4596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4666,7 +4669,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4739,7 +4742,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4812,7 +4815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4885,7 +4888,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4958,7 +4961,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -5031,7 +5034,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -5104,7 +5107,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -5177,7 +5180,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -5250,7 +5253,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -5323,7 +5326,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -5396,7 +5399,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -5536,7 +5539,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -5609,7 +5612,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -5682,7 +5685,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -5755,7 +5758,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -5828,7 +5831,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5974,7 +5977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -6041,7 +6044,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -6114,7 +6117,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -6187,7 +6190,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -6260,7 +6263,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -6333,7 +6336,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -6546,7 +6549,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -6619,7 +6622,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -6692,7 +6695,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -6765,7 +6768,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -6838,7 +6841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -6911,7 +6914,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -6978,7 +6981,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -7051,7 +7054,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -7124,7 +7127,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -7194,7 +7197,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -7340,7 +7343,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -7413,7 +7416,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -7486,7 +7489,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -7559,7 +7562,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -7632,7 +7635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -7705,7 +7708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -7772,7 +7775,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -7918,7 +7921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -7985,7 +7988,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
@@ -8058,7 +8061,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
@@ -8125,7 +8128,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
@@ -8192,7 +8195,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
@@ -8262,7 +8265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -8335,7 +8338,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
@@ -8405,7 +8408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
@@ -8472,7 +8475,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -8539,7 +8542,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -8609,7 +8612,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -8676,7 +8679,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -8746,7 +8749,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -8813,7 +8816,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
@@ -8880,7 +8883,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
@@ -8947,7 +8950,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
@@ -9020,7 +9023,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
@@ -9090,7 +9093,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
@@ -9163,7 +9166,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
@@ -9236,7 +9239,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
@@ -9303,7 +9306,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
@@ -9376,7 +9379,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
@@ -9449,7 +9452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
@@ -9522,7 +9525,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
@@ -9595,7 +9598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
@@ -9668,7 +9671,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
@@ -9741,7 +9744,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -9808,7 +9811,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
@@ -9881,7 +9884,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
@@ -9954,7 +9957,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
@@ -10027,7 +10030,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
@@ -10100,7 +10103,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
@@ -10133,6 +10136,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O245">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="user"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>